<commit_message>
[labb2] Namn på axlar på diagramen.
</commit_message>
<xml_diff>
--- a/Execution2.xlsx
+++ b/Execution2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="220" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="6780" yWindow="225" windowWidth="7500" windowHeight="4920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,24 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>NUM_THREADS</t>
   </si>
   <si>
     <t>Execution time</t>
-  </si>
-  <si>
-    <t>0.001902</t>
-  </si>
-  <si>
-    <t>0.002296</t>
-  </si>
-  <si>
-    <t>0.003488</t>
-  </si>
-  <si>
-    <t>0.004916</t>
   </si>
   <si>
     <t>Radius</t>
@@ -47,7 +35,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -98,19 +86,632 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Blurfilter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Radie 50</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.54347000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28952699999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23630999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22353700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.214757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.226544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23223099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26022800000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.31322100000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36029800000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.382185</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.38943100000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.45605400000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.53908699999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.52925199999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.55932999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.52662799999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Radie 500</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$20:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>4.5505800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.25936</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8264399999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5860799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.42171</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.31732</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2284999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1731199999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0203600000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1785800000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1985199999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1655000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5356999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.9739499999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.75406</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9392499999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.3780700000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5690999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="96891264"/>
+        <c:axId val="96892800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="96891264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Trådar</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96892800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96892800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Exekveringstid</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96891264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Thresholdfilter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>"Tresfilter"</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.902E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2959999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4880000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9160000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="39336576"/>
+        <c:axId val="39338368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="39336576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Trådar</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39338368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39338368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Exekveringstid</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39336576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,18 +1039,18 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B5" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,15 +1064,15 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>1.902E-3</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -483,12 +1084,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>2.2959999999999999E-3</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -500,12 +1101,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>3.4880000000000002E-3</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -517,12 +1118,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <v>4.9160000000000002E-3</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -534,7 +1135,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>5</v>
       </c>
@@ -545,7 +1146,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>6</v>
       </c>
@@ -556,7 +1157,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>7</v>
       </c>
@@ -567,7 +1168,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>8</v>
       </c>
@@ -578,7 +1179,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>9</v>
       </c>
@@ -589,7 +1190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>10</v>
       </c>
@@ -600,7 +1201,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>11</v>
       </c>
@@ -611,7 +1212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>12</v>
       </c>
@@ -622,7 +1223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>13</v>
       </c>
@@ -633,7 +1234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>14</v>
       </c>
@@ -644,7 +1245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>15</v>
       </c>
@@ -655,7 +1256,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>16</v>
       </c>
@@ -666,7 +1267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="4:6">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>17</v>
       </c>
@@ -677,7 +1278,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>18</v>
       </c>
@@ -688,7 +1289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>1</v>
       </c>
@@ -699,7 +1300,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>2</v>
       </c>
@@ -710,7 +1311,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="4:6">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>3</v>
       </c>
@@ -721,7 +1322,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="4:6">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>4</v>
       </c>
@@ -732,7 +1333,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="4:6">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>5</v>
       </c>
@@ -743,7 +1344,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="4:6">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>6</v>
       </c>
@@ -754,7 +1355,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="4:6">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>7</v>
       </c>
@@ -765,7 +1366,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="4:6">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>8</v>
       </c>
@@ -776,7 +1377,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="4:6">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>9</v>
       </c>
@@ -787,7 +1388,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="29" spans="4:6">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>10</v>
       </c>
@@ -798,7 +1399,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="30" spans="4:6">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>11</v>
       </c>
@@ -809,7 +1410,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="4:6">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>12</v>
       </c>
@@ -820,7 +1421,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="4:6">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>13</v>
       </c>
@@ -831,7 +1432,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="33" spans="4:6">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>14</v>
       </c>
@@ -842,7 +1443,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="34" spans="4:6">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>15</v>
       </c>
@@ -853,7 +1454,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="4:6">
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>16</v>
       </c>
@@ -864,7 +1465,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="4:6">
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>17</v>
       </c>
@@ -875,7 +1476,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="4:6">
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>18</v>
       </c>
@@ -889,6 +1490,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>